<commit_message>
Added more repos to replacements.txt file
</commit_message>
<xml_diff>
--- a/data/ACCESS_TOKEN_Input_File.xlsx
+++ b/data/ACCESS_TOKEN_Input_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\post-migration-self-service\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1A4F1E-EB47-4AB6-BA92-9250B79B64D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F378E77-23A2-4AC7-B06D-DB5E87C5696E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{8ADFF334-5768-4019-8CF1-F97373308AC5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="17">
   <si>
     <t>Repository</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>github-gk-aks/secondgithubrepo</t>
+  </si>
+  <si>
+    <t>github-gk-aks/thirdgithubrepo</t>
+  </si>
+  <si>
+    <t>github-gk-aks/fourthgithubrepo</t>
+  </si>
+  <si>
+    <t>github-gk-aks/fifthgithubrepo</t>
   </si>
 </sst>
 </file>
@@ -418,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB03B6E-AF43-4750-8C05-4678A6396883}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C12" sqref="C12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,6 +553,76 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>